<commit_message>
A1 writer wasn't printing, now it is
</commit_message>
<xml_diff>
--- a/workbookFinal.xlsx
+++ b/workbookFinal.xlsx
@@ -418,8 +418,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="B1:O1"/>
+  <dimension ref="A1:O1"/>
   <cols>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
@@ -436,7 +437,10 @@
     <col min="15" max="15" width="25.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="8" customFormat="1" ht="40" customHeight="1">
+    <row r="1" spans="1:15" s="8" customFormat="1" ht="40" customHeight="1">
+      <c r="A1" s="9" t="str">
+        <v>Band Name</v>
+      </c>
       <c r="B1" s="9" t="str">
         <v>Band Number</v>
       </c>

</xml_diff>